<commit_message>
mac terminal コマンド追加 #5
</commit_message>
<xml_diff>
--- a/004_技術資料/002_コマンド/コマンド一覧.xlsx
+++ b/004_技術資料/002_コマンド/コマンド一覧.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shotatsuji/work/document/share/document/004_技術資料/002_コマンド/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shotatsuji/work/doc/share/004_技術資料/002_コマンド/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F9D976-553E-7542-BA29-E8B4F40D95A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502E404F-9986-EE4D-AC71-7FE70000D870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cmd" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="104">
   <si>
     <t>番号</t>
     <rPh sb="0" eb="2">
@@ -641,6 +641,27 @@
     <t>zip [zipファイル名] [ファイル名]</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>[zipフォルダ名]に[フォルダ名]を暗号化する</t>
+    <rPh sb="8" eb="9">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="19" eb="22">
+      <t>アンゴウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ディレクトリ内のファイルを再帰的に扱う</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>zip ※1 [フォルダ名] [フォルダ名]/</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -898,6 +919,28 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8DB32F1A-3499-4EC1-A4B1-9ECFD7EA034C}" name="テーブル6" displayName="テーブル6" ref="F21:H22" totalsRowShown="0">
+  <autoFilter ref="F21:H22" xr:uid="{8DB32F1A-3499-4EC1-A4B1-9ECFD7EA034C}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0B9C9CFA-759F-4FB0-B0B9-668B5C6E9D43}" name="操作の説明" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{1652CC36-05BE-48F7-963B-4F9EB0368AD0}" name="操作方法"/>
+    <tableColumn id="3" xr3:uid="{309478A7-2D5A-44DF-8CDF-D38D5E7CA38F}" name="進捗"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9B23BEA6-8347-4451-918F-8EE7B55E0805}" name="テーブル7" displayName="テーブル7" ref="F24:F25" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="F24:F25" xr:uid="{9B23BEA6-8347-4451-918F-8EE7B55E0805}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{A4AD64F4-F204-4461-941E-B8F11E5C4647}" name="番号"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A51BD3D-0048-4E6E-BB0B-DC4FDAD4923E}" name="テーブル8" displayName="テーブル8" ref="F26:H27" totalsRowShown="0">
   <autoFilter ref="F26:H27" xr:uid="{0A51BD3D-0048-4E6E-BB0B-DC4FDAD4923E}"/>
   <tableColumns count="3">
@@ -909,7 +952,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C3E3DC82-5E5A-45A8-91C0-DC6634410869}" name="テーブル9" displayName="テーブル9" ref="F29:G30" totalsRowShown="0">
   <autoFilter ref="F29:G30" xr:uid="{C3E3DC82-5E5A-45A8-91C0-DC6634410869}"/>
   <tableColumns count="2">
@@ -920,7 +963,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{1D545E13-AF26-4B49-8E55-AD8B3FA5AB01}" name="テーブル10" displayName="テーブル10" ref="F31:H37" totalsRowShown="0">
   <autoFilter ref="F31:H37" xr:uid="{1D545E13-AF26-4B49-8E55-AD8B3FA5AB01}"/>
   <tableColumns count="3">
@@ -932,7 +975,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8818C13A-93F6-4718-97D1-8554F17B3306}" name="テーブル11" displayName="テーブル11" ref="F39:F40" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="F39:F40" xr:uid="{8818C13A-93F6-4718-97D1-8554F17B3306}"/>
   <tableColumns count="1">
@@ -942,7 +985,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{FD5DC2FF-A04E-4CF6-AC48-0E251F25270B}" name="テーブル12" displayName="テーブル12" ref="F41:H43" totalsRowShown="0">
   <autoFilter ref="F41:H43" xr:uid="{FD5DC2FF-A04E-4CF6-AC48-0E251F25270B}"/>
   <tableColumns count="3">
@@ -954,7 +997,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{F26FE757-2B1E-4CE5-92BC-700FA7EC36E1}" name="テーブル25" displayName="テーブル25" ref="F1:F2" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="F1:F2" xr:uid="{F26FE757-2B1E-4CE5-92BC-700FA7EC36E1}"/>
   <tableColumns count="1">
@@ -964,7 +1007,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{55111B81-DCE5-415C-9CE6-8EA0FE635F17}" name="テーブル26" displayName="テーブル26" ref="F3:H4" totalsRowShown="0">
   <autoFilter ref="F3:H4" xr:uid="{55111B81-DCE5-415C-9CE6-8EA0FE635F17}"/>
   <tableColumns count="3">
@@ -989,6 +1032,28 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BC0F620A-357E-F140-9853-DA65AE6B41C5}" name="テーブル15" displayName="テーブル15" ref="F1:F2" totalsRowShown="0">
+  <autoFilter ref="F1:F2" xr:uid="{BC0F620A-357E-F140-9853-DA65AE6B41C5}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{F6423084-5518-D545-B56E-F7DAE3B246A4}" name="番号"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{C7B3DD23-CAAC-8F42-99EA-FF4A9A191676}" name="テーブル17" displayName="テーブル17" ref="F3:H4" totalsRowShown="0">
+  <autoFilter ref="F3:H4" xr:uid="{C7B3DD23-CAAC-8F42-99EA-FF4A9A191676}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{F9EDF1C1-5C12-384B-901C-7B8B9BAB6275}" name="操作の説明"/>
+    <tableColumn id="2" xr3:uid="{EEAAC202-C8E8-3040-A953-B26643541420}" name="操作方法"/>
+    <tableColumn id="3" xr3:uid="{3328650D-F00C-B14A-B14C-76CF26281746}" name="進捗"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9C2F09C-A2DF-458A-9C62-44C6800CD98D}" name="テーブル1" displayName="テーブル1" ref="F1:F2" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="F1:F2" xr:uid="{C9C2F09C-A2DF-458A-9C62-44C6800CD98D}"/>
   <tableColumns count="1">
@@ -998,7 +1063,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BD85D786-2D44-47E0-894A-D2957F8AF4D3}" name="テーブル2" displayName="テーブル2" ref="F3:H5" totalsRowShown="0">
   <autoFilter ref="F3:H5" xr:uid="{BD85D786-2D44-47E0-894A-D2957F8AF4D3}"/>
   <tableColumns count="3">
@@ -1010,7 +1075,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E5B9642B-C26F-4ED4-A96C-FDCBB417075D}" name="テーブル3" displayName="テーブル3" ref="F7:F8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="F7:F8" xr:uid="{E5B9642B-C26F-4ED4-A96C-FDCBB417075D}"/>
   <tableColumns count="1">
@@ -1020,7 +1085,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4C9D06B7-E1DE-49B1-BF7E-34627FA59CB5}" name="テーブル4" displayName="テーブル4" ref="F9:H17" totalsRowShown="0">
   <autoFilter ref="F9:H17" xr:uid="{4C9D06B7-E1DE-49B1-BF7E-34627FA59CB5}"/>
   <tableColumns count="3">
@@ -1032,33 +1097,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A005A02C-A120-416B-ABD9-78F4A1D04E97}" name="テーブル5" displayName="テーブル5" ref="F19:F20" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="F19:F20" xr:uid="{A005A02C-A120-416B-ABD9-78F4A1D04E97}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{E818AB7C-586F-4A27-B0B1-5D660CB6BEC1}" name="番号"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8DB32F1A-3499-4EC1-A4B1-9ECFD7EA034C}" name="テーブル6" displayName="テーブル6" ref="F21:H22" totalsRowShown="0">
-  <autoFilter ref="F21:H22" xr:uid="{8DB32F1A-3499-4EC1-A4B1-9ECFD7EA034C}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0B9C9CFA-759F-4FB0-B0B9-668B5C6E9D43}" name="操作の説明" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{1652CC36-05BE-48F7-963B-4F9EB0368AD0}" name="操作方法"/>
-    <tableColumn id="3" xr3:uid="{309478A7-2D5A-44DF-8CDF-D38D5E7CA38F}" name="進捗"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9B23BEA6-8347-4451-918F-8EE7B55E0805}" name="テーブル7" displayName="テーブル7" ref="F24:F25" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="F24:F25" xr:uid="{9B23BEA6-8347-4451-918F-8EE7B55E0805}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A4AD64F4-F204-4461-941E-B8F11E5C4647}" name="番号"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3879,7 +3922,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997F91C-B6FE-6C41-9B99-32BF76E2ECD8}">
-  <dimension ref="A1:D301"/>
+  <dimension ref="A1:H301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3889,9 +3932,11 @@
     <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3904,8 +3949,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3918,8 +3966,11 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3932,16 +3983,40 @@
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3949,7 +4024,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3957,7 +4032,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3965,7 +4040,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3973,7 +4048,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3981,7 +4056,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3989,7 +4064,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3997,7 +4072,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4005,7 +4080,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4013,7 +4088,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4021,7 +4096,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4029,7 +4104,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -6320,12 +6395,16 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D301" xr:uid="{4212AFE7-676F-4A4A-9028-1F4A8A1E7E8D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D301 H4" xr:uid="{4212AFE7-676F-4A4A-9028-1F4A8A1E7E8D}">
       <formula1>"open,close"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>